<commit_message>
Fixing an error Sacha identified
</commit_message>
<xml_diff>
--- a/metadata/Diel_RNA_sample_metadata.xlsx
+++ b/metadata/Diel_RNA_sample_metadata.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrco/Code/DielPAR/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8BAE631B-B06C-F340-B197-BAABF398A341}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37900" yWindow="380" windowWidth="29120" windowHeight="19080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Diel_RNA_sample_metadata" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,15 @@
   <definedNames>
     <definedName name="_GoBack" localSheetId="0">Diel_RNA_sample_metadata!$E$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -253,9 +260,6 @@
     <t>2015-07-29T10:00:00-10:00</t>
   </si>
   <si>
-    <t>2015-07-29T22:25:00-00:00</t>
-  </si>
-  <si>
     <t>2015-07-29T14:00:00-10:00</t>
   </si>
   <si>
@@ -359,12 +363,15 @@
   </si>
   <si>
     <t>Cast_no</t>
+  </si>
+  <si>
+    <t>2015-07-29T20:25:00-00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1208,11 +1215,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1244,27 +1251,27 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
         <v>110</v>
-      </c>
-      <c r="C4" t="s">
-        <v>111</v>
       </c>
       <c r="D4" t="s">
         <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
         <v>85</v>
-      </c>
-      <c r="G4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -1273,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="1">
         <v>6</v>
@@ -1287,7 +1294,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -1296,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="1">
         <v>6</v>
@@ -1319,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="1">
         <v>10</v>
@@ -1342,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" s="1">
         <v>10</v>
@@ -1365,7 +1372,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="1">
         <v>14</v>
@@ -1388,7 +1395,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" s="1">
         <v>14</v>
@@ -1411,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="1">
         <v>18</v>
@@ -1434,7 +1441,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E12" s="1">
         <v>18</v>
@@ -1457,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" s="1">
         <v>22</v>
@@ -1480,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E14" s="1">
         <v>22</v>
@@ -1494,7 +1501,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15">
         <v>15</v>
@@ -1503,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="1">
         <v>26</v>
@@ -1517,7 +1524,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1526,7 +1533,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" s="1">
         <v>26</v>
@@ -1540,7 +1547,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1549,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E17" s="1">
         <v>30</v>
@@ -1563,7 +1570,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -1572,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E18" s="1">
         <v>30</v>
@@ -1595,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E19" s="1">
         <v>34</v>
@@ -1618,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E20" s="1">
         <v>34</v>
@@ -1641,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E21" s="1">
         <v>38</v>
@@ -1664,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" s="1">
         <v>38</v>
@@ -1687,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E23" s="1">
         <v>42</v>
@@ -1710,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" s="1">
         <v>42</v>
@@ -1733,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E25" s="1">
         <v>46</v>
@@ -1756,7 +1763,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26" s="1">
         <v>46</v>
@@ -1770,7 +1777,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B27">
         <v>21</v>
@@ -1779,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E27" s="1">
         <v>50</v>
@@ -1793,7 +1800,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28">
         <v>21</v>
@@ -1802,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E28" s="1">
         <v>50</v>
@@ -1816,7 +1823,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29">
         <v>22</v>
@@ -1825,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E29" s="1">
         <v>54</v>
@@ -1839,7 +1846,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30">
         <v>22</v>
@@ -1848,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E30" s="1">
         <v>54</v>
@@ -1871,7 +1878,7 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E31" s="1">
         <v>58</v>
@@ -1894,7 +1901,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E32" s="1">
         <v>58</v>
@@ -1917,7 +1924,7 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E33" s="1">
         <v>62</v>
@@ -1940,7 +1947,7 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" s="1">
         <v>62</v>
@@ -1963,7 +1970,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E35" s="1">
         <v>66</v>
@@ -1986,7 +1993,7 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E36" s="1">
         <v>66</v>
@@ -2009,7 +2016,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E37" s="1">
         <v>70</v>
@@ -2032,7 +2039,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E38" s="1">
         <v>70</v>
@@ -2046,7 +2053,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B39">
         <v>29</v>
@@ -2055,7 +2062,7 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E39" s="1">
         <v>74</v>
@@ -2069,7 +2076,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B40">
         <v>29</v>
@@ -2078,7 +2085,7 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E40" s="1">
         <v>74</v>
@@ -2092,7 +2099,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41">
         <v>30</v>
@@ -2101,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E41" s="1">
         <v>78</v>
@@ -2115,7 +2122,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B42">
         <v>30</v>
@@ -2124,7 +2131,7 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E42" s="1">
         <v>78</v>
@@ -2147,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E43" s="1">
         <v>82</v>
@@ -2156,7 +2163,7 @@
         <v>75</v>
       </c>
       <c r="G43" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2170,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E44" s="1">
         <v>82</v>
@@ -2179,7 +2186,7 @@
         <v>75</v>
       </c>
       <c r="G44" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2193,16 +2200,16 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E45" s="1">
         <v>86</v>
       </c>
       <c r="F45" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" t="s">
         <v>77</v>
-      </c>
-      <c r="G45" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -2216,16 +2223,16 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E46" s="1">
         <v>86</v>
       </c>
       <c r="F46" t="s">
+        <v>76</v>
+      </c>
+      <c r="G46" t="s">
         <v>77</v>
-      </c>
-      <c r="G46" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2239,16 +2246,16 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E47" s="1">
         <v>90</v>
       </c>
       <c r="F47" t="s">
+        <v>78</v>
+      </c>
+      <c r="G47" t="s">
         <v>79</v>
-      </c>
-      <c r="G47" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2262,16 +2269,16 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E48" s="1">
         <v>90</v>
       </c>
       <c r="F48" t="s">
+        <v>78</v>
+      </c>
+      <c r="G48" t="s">
         <v>79</v>
-      </c>
-      <c r="G48" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -2285,16 +2292,16 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E49" s="1">
         <v>94</v>
       </c>
       <c r="F49" t="s">
+        <v>80</v>
+      </c>
+      <c r="G49" t="s">
         <v>81</v>
-      </c>
-      <c r="G49" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2308,21 +2315,21 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E50" s="1">
         <v>94</v>
       </c>
       <c r="F50" t="s">
+        <v>80</v>
+      </c>
+      <c r="G50" t="s">
         <v>81</v>
-      </c>
-      <c r="G50" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B51">
         <v>35</v>
@@ -2331,21 +2338,21 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E51" s="1">
         <v>98</v>
       </c>
       <c r="F51" t="s">
+        <v>82</v>
+      </c>
+      <c r="G51" t="s">
         <v>83</v>
-      </c>
-      <c r="G51" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B52">
         <v>35</v>
@@ -2354,16 +2361,16 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E52" s="1">
         <v>98</v>
       </c>
       <c r="F52" t="s">
+        <v>82</v>
+      </c>
+      <c r="G52" t="s">
         <v>83</v>
-      </c>
-      <c r="G52" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing how the timezone appears in the ISO timestamps
</commit_message>
<xml_diff>
--- a/metadata/Diel_RNA_sample_metadata.xlsx
+++ b/metadata/Diel_RNA_sample_metadata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrco/Code/DielPAR/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{13B2274E-F8A5-1344-B55F-997DCAB8D530}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="36300" yWindow="-360" windowWidth="28800" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diel_RNA_sample_metadata" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_GoBack" localSheetId="0">Diel_RNA_sample_metadata!$E$5</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -143,147 +144,6 @@
     <t>Cruise KM1513 was the SCOPE HOE-Legacy 2A cruise; exact bottle closure times gathered by Sacha from CTD tearsheets</t>
   </si>
   <si>
-    <t>2015-07-26T10:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-26T06:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-26T17:11:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-26T20:25:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-26T14:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T00:29:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-26T18:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T04:27:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-26T22:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T08:46:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T02:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T12:27:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T06:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T16:26:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T10:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T20:23:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T14:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T00:41:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T18:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T04:35:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-27T22:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T08:28:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T02:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T12:30:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T06:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T16:24:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T10:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T20:19:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T14:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T00:33:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T18:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T04:37:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-28T22:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T08:26:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T02:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T12:31:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T06:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T16:24:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T10:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T14:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-30T00:26:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T18:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-30T04:30:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-29T22:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-30T08:15:00-00:00</t>
-  </si>
-  <si>
-    <t>2015-07-30T02:00:00-10:00</t>
-  </si>
-  <si>
-    <t>2015-07-30T12:28:00-00:00</t>
-  </si>
-  <si>
     <t>Timestamp_nominal_HST_ISO8601</t>
   </si>
   <si>
@@ -365,13 +225,154 @@
     <t>Cast_no</t>
   </si>
   <si>
-    <t>2015-07-29T20:25:00-00:00</t>
+    <t>2015-07-26T06:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-26T10:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-26T17:11:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-26T20:25:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-26T14:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-27T00:29:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-26T18:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-27T04:27:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-26T22:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-27T08:46:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-27T02:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-27T12:27:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-27T06:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-27T16:26:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-27T10:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-27T20:23:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-27T14:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-28T00:41:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-27T18:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-28T04:35:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-27T22:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-28T08:28:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-28T02:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-28T12:30:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-28T06:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-28T16:24:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-28T10:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-28T20:19:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-28T14:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-29T00:33:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-28T18:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-29T04:37:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-28T22:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-29T08:26:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-29T02:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-29T12:31:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-29T06:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-29T16:24:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-29T10:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-29T20:25:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-29T14:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-30T00:26:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-29T18:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-30T04:30:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-29T22:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-30T08:15:00-0000</t>
+  </si>
+  <si>
+    <t>2015-07-30T02:00:00-1000</t>
+  </si>
+  <si>
+    <t>2015-07-30T12:28:00-0000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1215,11 +1216,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1251,27 +1252,27 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
         <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -1280,21 +1281,21 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1">
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -1303,16 +1304,16 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1326,16 +1327,16 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E7" s="1">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1349,16 +1350,16 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1372,16 +1373,16 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1395,16 +1396,16 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1418,16 +1419,16 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1">
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1441,16 +1442,16 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1">
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1464,16 +1465,16 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E13" s="1">
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1487,21 +1488,21 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E14" s="1">
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>15</v>
@@ -1510,21 +1511,21 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E15" s="1">
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1533,21 +1534,21 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E16" s="1">
         <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="G16" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1556,21 +1557,21 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1">
         <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="G17" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -1579,16 +1580,16 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="E18" s="1">
         <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1602,16 +1603,16 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E19" s="1">
         <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1625,16 +1626,16 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E20" s="1">
         <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1648,16 +1649,16 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E21" s="1">
         <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1671,16 +1672,16 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1">
         <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="G22" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1694,16 +1695,16 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E23" s="1">
         <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1717,16 +1718,16 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E24" s="1">
         <v>42</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="G24" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1740,16 +1741,16 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E25" s="1">
         <v>46</v>
       </c>
       <c r="F25" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1763,21 +1764,21 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E26" s="1">
         <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="G26" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>55</v>
       </c>
       <c r="B27">
         <v>21</v>
@@ -1786,21 +1787,21 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E27" s="1">
         <v>50</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="B28">
         <v>21</v>
@@ -1809,21 +1810,21 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E28" s="1">
         <v>50</v>
       </c>
       <c r="F28" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="G28" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="B29">
         <v>22</v>
@@ -1832,21 +1833,21 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="E29" s="1">
         <v>54</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="G29" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="B30">
         <v>22</v>
@@ -1855,16 +1856,16 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="E30" s="1">
         <v>54</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="G30" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1878,16 +1879,16 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E31" s="1">
         <v>58</v>
       </c>
       <c r="F31" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="G31" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1901,16 +1902,16 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E32" s="1">
         <v>58</v>
       </c>
       <c r="F32" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="G32" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1924,16 +1925,16 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E33" s="1">
         <v>62</v>
       </c>
       <c r="F33" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="G33" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1947,16 +1948,16 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E34" s="1">
         <v>62</v>
       </c>
       <c r="F34" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="G34" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1970,16 +1971,16 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E35" s="1">
         <v>66</v>
       </c>
       <c r="F35" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="G35" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1993,16 +1994,16 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E36" s="1">
         <v>66</v>
       </c>
       <c r="F36" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="G36" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2016,16 +2017,16 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E37" s="1">
         <v>70</v>
       </c>
       <c r="F37" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="G37" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -2039,21 +2040,21 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E38" s="1">
         <v>70</v>
       </c>
       <c r="F38" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="G38" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="B39">
         <v>29</v>
@@ -2062,21 +2063,21 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E39" s="1">
         <v>74</v>
       </c>
       <c r="F39" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="G39" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="B40">
         <v>29</v>
@@ -2085,21 +2086,21 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E40" s="1">
         <v>74</v>
       </c>
       <c r="F40" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="G40" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="B41">
         <v>30</v>
@@ -2108,21 +2109,21 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1">
         <v>78</v>
       </c>
       <c r="F41" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="G41" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="B42">
         <v>30</v>
@@ -2131,16 +2132,16 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="E42" s="1">
         <v>78</v>
       </c>
       <c r="F42" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="G42" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2154,16 +2155,16 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E43" s="1">
         <v>82</v>
       </c>
       <c r="F43" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="G43" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2177,16 +2178,16 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E44" s="1">
         <v>82</v>
       </c>
       <c r="F44" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="G44" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2200,16 +2201,16 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E45" s="1">
         <v>86</v>
       </c>
       <c r="F45" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="G45" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -2223,16 +2224,16 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E46" s="1">
         <v>86</v>
       </c>
       <c r="F46" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="G46" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2246,16 +2247,16 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E47" s="1">
         <v>90</v>
       </c>
       <c r="F47" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="G47" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2269,16 +2270,16 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E48" s="1">
         <v>90</v>
       </c>
       <c r="F48" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="G48" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -2292,16 +2293,16 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E49" s="1">
         <v>94</v>
       </c>
       <c r="F49" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="G49" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2315,21 +2316,21 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E50" s="1">
         <v>94</v>
       </c>
       <c r="F50" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="G50" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="B51">
         <v>35</v>
@@ -2338,21 +2339,21 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E51" s="1">
         <v>98</v>
       </c>
       <c r="F51" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="G51" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="B52">
         <v>35</v>
@@ -2361,16 +2362,16 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E52" s="1">
         <v>98</v>
       </c>
       <c r="F52" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="G52" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>